<commit_message>
la concha de tu madre all boys
</commit_message>
<xml_diff>
--- a/E2EUAT.xlsx
+++ b/E2EUAT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto Fan\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="288">
   <si>
     <t>Descripción</t>
   </si>
@@ -874,6 +874,18 @@
   </si>
   <si>
     <t>RecargaHistoria</t>
+  </si>
+  <si>
+    <t>packDe1dIaPersonal</t>
+  </si>
+  <si>
+    <t>22225062</t>
+  </si>
+  <si>
+    <t>2932550231</t>
+  </si>
+  <si>
+    <t>Pack SMS y Minutos a Personal Ilimitados x 1 día</t>
   </si>
 </sst>
 </file>
@@ -3262,7 +3274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -4126,10 +4138,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4426,26 +4438,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
-        <v>228</v>
+        <v>284</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>189</v>
+        <v>285</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>54</v>
+        <v>286</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>287</v>
       </c>
       <c r="E10" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="79" t="s">
         <v>229</v>
       </c>
       <c r="H10" s="21" t="s">
@@ -4472,28 +4484,27 @@
       <c r="O10" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="1:27" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:27" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>274</v>
+        <v>189</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="D11" s="79" t="s">
-        <v>276</v>
+        <v>190</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="E11" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="78" t="s">
         <v>229</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -4522,9 +4533,9 @@
       </c>
       <c r="P11" s="19"/>
     </row>
-    <row r="12" spans="1:27" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" s="79" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>188</v>
+        <v>273</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>274</v>
@@ -4532,25 +4543,47 @@
       <c r="C12" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>192</v>
+      <c r="D12" s="79" t="s">
+        <v>276</v>
       </c>
       <c r="E12" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>100</v>
+      <c r="G12" s="79" t="s">
+        <v>229</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+      <c r="I12" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="1:27" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>274</v>
@@ -4574,95 +4607,98 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="79" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G15" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J15" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K15" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L15" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M15" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="N15" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="O14" s="14"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-    </row>
-    <row r="15" spans="1:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>236</v>
-      </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="36"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
     </row>
     <row r="16" spans="1:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="D16" s="69"/>
       <c r="E16" s="46"/>
@@ -4677,194 +4713,217 @@
       <c r="N16" s="35"/>
       <c r="O16" s="36"/>
     </row>
-    <row r="17" spans="1:27" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="69"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="36"/>
+    </row>
+    <row r="18" spans="1:27" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B18" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="D17" s="80" t="s">
+      <c r="D18" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="E17" s="83" t="s">
+      <c r="E18" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="80" t="s">
+      <c r="F18" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="80" t="s">
+      <c r="G18" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="H17" s="81" t="s">
+      <c r="H18" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="80" t="s">
+      <c r="I18" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="J17" s="84" t="s">
+      <c r="J18" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="K17" s="80" t="s">
+      <c r="K18" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="82" t="s">
+      <c r="L18" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N17" s="82" t="s">
+      <c r="N18" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="O18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="P18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q18" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="R17" s="96" t="s">
+      <c r="R18" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="S17" s="96"/>
-    </row>
-    <row r="18" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="S18" s="96"/>
+    </row>
+    <row r="19" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C19" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D19" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G19" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H19" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I19" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K19" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="L18" s="14" t="s">
+      <c r="L19" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M19" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="N18" s="14" t="s">
+      <c r="N19" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="O18" s="14"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-    </row>
-    <row r="19" spans="1:27" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" s="61" t="s">
-        <v>279</v>
-      </c>
-      <c r="D19" s="61"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
     </row>
     <row r="20" spans="1:27" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" s="61"/>
+    </row>
+    <row r="21" spans="1:27" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="C20" s="94">
+      <c r="C21" s="94">
         <v>2944675128</v>
       </c>
-      <c r="D20" s="61"/>
-    </row>
-    <row r="21" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="D21" s="61"/>
+    </row>
+    <row r="22" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C22" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D22" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E22" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F22" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H22" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I22" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J22" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="34" t="s">
+      <c r="K22" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L22" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="18" t="s">
+      <c r="M22" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N21" s="18" t="s">
+      <c r="N22" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C24" s="95"/>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="C25" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>